<commit_message>
Subida completa del proyecto
</commit_message>
<xml_diff>
--- a/results/domain_comparison_filter.xlsx
+++ b/results/domain_comparison_filter.xlsx
@@ -50,37 +50,43 @@
     <t xml:space="preserve">Fibronectin type 3 domain</t>
   </si>
   <si>
+    <t xml:space="preserve">Ig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Immunoglobulin domain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COG1100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KRAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GTPase SAR1 and related small G proteins [General function prediction only]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CUB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CUB domain</t>
+  </si>
+  <si>
     <t xml:space="preserve">I-set</t>
   </si>
   <si>
     <t xml:space="preserve">Immunoglobulin I-set domain</t>
   </si>
   <si>
-    <t xml:space="preserve">Ig</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Immunoglobulin domain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COG1100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KRAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GTPase SAR1 and related small G proteins [General function prediction only]</t>
-  </si>
-  <si>
     <t xml:space="preserve">LamG</t>
   </si>
   <si>
     <t xml:space="preserve">Laminin G domain</t>
   </si>
   <si>
-    <t xml:space="preserve">CUB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CUB domain</t>
+    <t xml:space="preserve">Ion_trans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ion transport protein</t>
   </si>
   <si>
     <t xml:space="preserve">COG2319</t>
@@ -89,24 +95,12 @@
     <t xml:space="preserve">FOG: WD40 repeat [General function prediction only]</t>
   </si>
   <si>
-    <t xml:space="preserve">Ion_trans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ion transport protein</t>
-  </si>
-  <si>
     <t xml:space="preserve">LRR_RI</t>
   </si>
   <si>
     <t xml:space="preserve">Leucine-rich repeats (LRRs), ribonuclease inhibitor (RI)-like subfamily. LRRs are 20-29 residue sequence motifs present in many proteins that participate in protein-protein interactions and have different functions and cellular locations. LRRs correspond...</t>
   </si>
   <si>
-    <t xml:space="preserve">SPEC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spectrin repeats, found in several proteins involved in cytoskeletal structure</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tryp_SPc</t>
   </si>
   <si>
@@ -131,24 +125,30 @@
     <t xml:space="preserve">Serine/Threonine protein kinases, catalytic domain</t>
   </si>
   <si>
+    <t xml:space="preserve">LIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cation transporter family protein</t>
+  </si>
+  <si>
     <t xml:space="preserve">EGF_CA</t>
   </si>
   <si>
     <t xml:space="preserve">Calcium-binding EGF-like domain, present in a large number of membrane-bound and extracellular (mostly animal) proteins. Many of these proteins require calcium for their biological function and calcium-binding sites have been found to be located at the...</t>
   </si>
   <si>
-    <t xml:space="preserve">LIC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cation transporter family protein</t>
-  </si>
-  <si>
     <t xml:space="preserve">PTPc</t>
   </si>
   <si>
     <t xml:space="preserve">Protein tyrosine phosphatases (PTP) catalyze the dephosphorylation of phosphotyrosine peptides</t>
   </si>
   <si>
+    <t xml:space="preserve">MYSc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Myosin. Large ATPases</t>
+  </si>
+  <si>
     <t xml:space="preserve">PTKc_EGFR</t>
   </si>
   <si>
@@ -164,12 +164,6 @@
     <t xml:space="preserve">WD40 domain, found in a number of eukaryotic proteins that cover a wide variety of functions including adaptor/regulatory modules in signal transduction, pre-mRNA processing and cytoskeleton assembly</t>
   </si>
   <si>
-    <t xml:space="preserve">MYSc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Myosin. Large ATPases</t>
-  </si>
-  <si>
     <t xml:space="preserve">P53</t>
   </si>
   <si>
@@ -180,6 +174,12 @@
   </si>
   <si>
     <t xml:space="preserve">PDZ domain found in a variety of Eumetazoan signaling molecules, often in tandem arrangements. May be responsible for specific protein-protein interactions, as most PDZ domains bind C-terminal polypeptides, and binding to internal (non-C-terminal)...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zf-H2C2_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zinc-finger double domain</t>
   </si>
 </sst>
 </file>
@@ -582,18 +582,18 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
@@ -692,7 +692,7 @@
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C17" t="s">
         <v>36</v>
@@ -703,7 +703,7 @@
         <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C18" t="s">
         <v>38</v>
@@ -714,7 +714,7 @@
         <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C19" t="s">
         <v>40</v>
@@ -725,7 +725,7 @@
         <v>41</v>
       </c>
       <c r="B20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C20" t="s">
         <v>42</v>
@@ -736,7 +736,7 @@
         <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C21" t="s">
         <v>44</v>

</xml_diff>